<commit_message>
Tests Succesful on Excel Read
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -299,7 +299,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed the bug that was sending two passwords that caused the test to fail
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -31,7 +31,23 @@
     <t xml:space="preserve">arrennbaral@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">djgjhsgksdgjo</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2kWip@HgY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">!S9gAL</t>
+    </r>
   </si>
   <si>
     <r>
@@ -66,25 +82,6 @@
   </si>
   <si>
     <t xml:space="preserve">3535osnd</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2kWip@HgY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">!S9gAL</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -299,7 +296,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -320,7 +317,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -353,16 +350,17 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="arrennbaral@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="arbaral@gil"/>
-    <hyperlink ref="A5" r:id="rId3" display="azz@gokg.com"/>
-    <hyperlink ref="A6" r:id="rId4" display="arrennbaral@gmail.com"/>
-    <hyperlink ref="B6" r:id="rId5" display="2kWip@HgY"/>
+    <hyperlink ref="B2" r:id="rId2" display="2kWip@HgY"/>
+    <hyperlink ref="A3" r:id="rId3" display="arbaral@gil"/>
+    <hyperlink ref="A5" r:id="rId4" display="azz@gokg.com"/>
+    <hyperlink ref="A6" r:id="rId5" display="arrennbaral@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId6" display="2kWip@HgY"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>